<commit_message>
ultimo cambios input form
</commit_message>
<xml_diff>
--- a/export_compras.xlsx
+++ b/export_compras.xlsx
@@ -15,18 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Numero Cot.</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Vendedor</t>
+    <t>Numero Doc.</t>
+  </si>
+  <si>
+    <t>Autorizacion</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -50,46 +50,34 @@
     <t>Estado Pago</t>
   </si>
   <si>
-    <t>Aprobado</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
-    <t>John Davis</t>
-  </si>
-  <si>
-    <t>2023-08-13</t>
-  </si>
-  <si>
-    <t>$39.20</t>
-  </si>
-  <si>
-    <t>$0.80</t>
-  </si>
-  <si>
-    <t>$4.70</t>
-  </si>
-  <si>
-    <t>$43.90</t>
-  </si>
-  <si>
-    <t>$44.80</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
+    <t>123-232-323232323</t>
+  </si>
+  <si>
+    <t>qweqwe</t>
+  </si>
+  <si>
+    <t>2023-08-22</t>
+  </si>
+  <si>
+    <t>$8610.00</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$1033.20</t>
+  </si>
+  <si>
+    <t>$9643.20</t>
+  </si>
+  <si>
+    <t>Pagado</t>
   </si>
   <si>
     <t>Activo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CABRERA GUEVARA RUDIGER ALEXY</t>
-  </si>
-  <si>
-    <t>$5.50</t>
-  </si>
-  <si>
-    <t>$0.00</t>
   </si>
 </sst>
 </file>
@@ -429,7 +417,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,11 +425,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="true" style="0"/>
-    <col min="3" max="3" width="20" customWidth="true" style="0"/>
-    <col min="4" max="4" width="20" customWidth="true" style="0"/>
-    <col min="5" max="5" width="11" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13" customWidth="true" style="0"/>
+    <col min="4" max="4" width="35" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10" customWidth="true" style="0"/>
+    <col min="6" max="6" width="14" customWidth="true" style="0"/>
     <col min="7" max="7" width="14" customWidth="true" style="0"/>
     <col min="8" max="8" width="14" customWidth="true" style="0"/>
     <col min="9" max="9" width="14" customWidth="true" style="0"/>
@@ -449,7 +437,7 @@
     <col min="11" max="11" width="12" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,19 +474,16 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2">
+        <v>12345678901</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -519,57 +504,13 @@
         <v>18</v>
       </c>
       <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
       <c r="L2" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>